<commit_message>
Entered values for the multiplier vector
Values entered to just do some testing on the conept.
</commit_message>
<xml_diff>
--- a/Multiplier.xlsx
+++ b/Multiplier.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
-  <si>
-    <t>N/A</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Body Ache</t>
   </si>
@@ -200,6 +197,39 @@
   </si>
   <si>
     <t>Rectum Pain</t>
+  </si>
+  <si>
+    <t>Anemia</t>
+  </si>
+  <si>
+    <t>Asthma</t>
+  </si>
+  <si>
+    <t>Cataracts</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <t>Cold Sore</t>
+  </si>
+  <si>
+    <t>Crohn's Disorder</t>
+  </si>
+  <si>
+    <t>Diabetes Type I</t>
+  </si>
+  <si>
+    <t>Flu</t>
+  </si>
+  <si>
+    <t>HIV</t>
+  </si>
+  <si>
+    <t>Meningitis</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -547,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK1"/>
+  <dimension ref="A1:BK11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -560,193 +590,429 @@
   <sheetData>
     <row r="1" spans="1:63" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
         <v>4</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="D2" s="2">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2">
+        <v>22</v>
+      </c>
+      <c r="M2" s="2">
+        <v>24</v>
+      </c>
+      <c r="N2" s="2">
+        <v>26</v>
+      </c>
+      <c r="O2" s="2">
+        <v>28</v>
+      </c>
+      <c r="P2" s="2">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>32</v>
+      </c>
+      <c r="R2" s="2">
         <v>34</v>
       </c>
-      <c r="AK1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" s="1" t="s">
+      <c r="S2" s="2">
         <v>36</v>
       </c>
-      <c r="AM1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN1" s="1" t="s">
+      <c r="T2" s="2">
         <v>38</v>
       </c>
-      <c r="AO1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP1" s="1" t="s">
+      <c r="U2" s="2">
         <v>40</v>
       </c>
-      <c r="AQ1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR1" s="1" t="s">
+      <c r="V2" s="2">
         <v>42</v>
       </c>
-      <c r="AS1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT1" s="1" t="s">
+      <c r="W2" s="2">
         <v>44</v>
       </c>
-      <c r="AU1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV1" s="1" t="s">
+      <c r="X2" s="2">
         <v>46</v>
       </c>
-      <c r="AW1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AX1" s="1" t="s">
+      <c r="Y2" s="2">
         <v>48</v>
       </c>
-      <c r="AY1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="Z2" s="2">
         <v>50</v>
       </c>
-      <c r="BA1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB1" s="1" t="s">
+      <c r="AA2" s="2">
         <v>52</v>
       </c>
-      <c r="BC1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BD1" s="1" t="s">
+      <c r="AB2" s="2">
         <v>54</v>
       </c>
-      <c r="BE1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BF1" s="1" t="s">
+      <c r="AC2" s="2">
         <v>56</v>
       </c>
-      <c r="BG1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BH1" s="1" t="s">
+      <c r="AD2" s="2">
         <v>58</v>
       </c>
-      <c r="BI1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="AE2" s="2">
         <v>60</v>
       </c>
-      <c r="BK1" s="1" t="s">
-        <v>61</v>
+      <c r="AF2" s="2">
+        <v>62</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>64</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>66</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>68</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>70</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>72</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>78</v>
+      </c>
+      <c r="AO2" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP2" s="2">
+        <v>82</v>
+      </c>
+      <c r="AQ2" s="2">
+        <v>84</v>
+      </c>
+      <c r="AR2" s="2">
+        <v>86</v>
+      </c>
+      <c r="AS2" s="2">
+        <v>88</v>
+      </c>
+      <c r="AT2" s="2">
+        <v>90</v>
+      </c>
+      <c r="AU2" s="2">
+        <v>92</v>
+      </c>
+      <c r="AV2" s="2">
+        <v>94</v>
+      </c>
+      <c r="AW2" s="2">
+        <v>96</v>
+      </c>
+      <c r="AX2" s="2">
+        <v>98</v>
+      </c>
+      <c r="AY2" s="2">
+        <v>100</v>
+      </c>
+      <c r="AZ2" s="2">
+        <v>102</v>
+      </c>
+      <c r="BA2" s="2">
+        <v>104</v>
+      </c>
+      <c r="BB2" s="2">
+        <v>106</v>
+      </c>
+      <c r="BC2" s="2">
+        <v>108</v>
+      </c>
+      <c r="BD2" s="2">
+        <v>110</v>
+      </c>
+      <c r="BE2" s="2">
+        <v>112</v>
+      </c>
+      <c r="BF2" s="2">
+        <v>114</v>
+      </c>
+      <c r="BG2" s="2">
+        <v>116</v>
+      </c>
+      <c r="BH2" s="2">
+        <v>118</v>
+      </c>
+      <c r="BI2" s="2">
+        <v>120</v>
+      </c>
+      <c r="BJ2" s="2">
+        <v>122</v>
+      </c>
+      <c r="BK2" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>